<commit_message>
adiciona fonte das kbas e areas do pat
</commit_message>
<xml_diff>
--- a/app/planilhas/fonte_dados.xlsx
+++ b/app/planilhas/fonte_dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SIG\RAN_homeoffice\PANs\Nordeste\ameacas_ne_rhino\app\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB6E386-6F8B-4BBC-908D-1B33DD09397A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EA15A2-1362-47CC-81FA-0C2254980875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{AC355D62-1078-4424-A2C4-A154FC936A63}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="69">
   <si>
     <t>Camada</t>
   </si>
@@ -189,18 +189,9 @@
     <t>Biomas</t>
   </si>
   <si>
-    <t>Áreas - PAT</t>
-  </si>
-  <si>
     <t>KBAs</t>
   </si>
   <si>
-    <t>Labels</t>
-  </si>
-  <si>
-    <t>Texto</t>
-  </si>
-  <si>
     <t>IBGE</t>
   </si>
   <si>
@@ -238,6 +229,21 @@
   </si>
   <si>
     <t>Limites</t>
+  </si>
+  <si>
+    <t>http://www.inema.ba.gov.br/plano-de-acao-territorial-pat-chapada-diamantina-serra-da-jiboia/</t>
+  </si>
+  <si>
+    <t>Áreas - PAT (Plano de Ação Territorial Chapada Diamantina-Serra da Jiboia)</t>
+  </si>
+  <si>
+    <t>INEMA/BA</t>
+  </si>
+  <si>
+    <t>https://www.keybiodiversityareas.org/</t>
+  </si>
+  <si>
+    <t>Key Biodiversity Area Partnership</t>
   </si>
 </sst>
 </file>
@@ -601,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC17CF5-4A4A-4110-9DC4-7CDD2145D379}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,7 +665,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -689,7 +695,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -718,7 +724,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -747,7 +753,7 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -776,7 +782,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
@@ -800,7 +806,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
@@ -823,7 +829,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
@@ -846,7 +852,7 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -875,7 +881,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
@@ -898,7 +904,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -921,7 +927,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -944,7 +950,7 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -967,7 +973,7 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
@@ -990,7 +996,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
         <v>39</v>
@@ -1013,16 +1019,16 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E16">
         <v>2021</v>
       </c>
       <c r="H16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I16" s="4">
         <v>44859</v>
@@ -1036,16 +1042,16 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I17" s="4">
         <v>45028</v>
@@ -1059,16 +1065,16 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E18">
         <v>2023</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I18" s="4">
         <v>45006</v>
@@ -1082,16 +1088,16 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E19">
         <v>2021</v>
       </c>
       <c r="H19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I19" s="4"/>
     </row>
@@ -1103,7 +1109,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
         <v>32</v>
@@ -1112,7 +1118,7 @@
         <v>2019</v>
       </c>
       <c r="H20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I20" s="4">
         <v>45007</v>
@@ -1126,16 +1132,16 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E21">
         <v>2019</v>
       </c>
       <c r="H21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I21" s="4">
         <v>44089</v>
@@ -1143,35 +1149,42 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
         <v>66</v>
+      </c>
+      <c r="E22">
+        <v>2020</v>
+      </c>
+      <c r="H22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I23" s="4">
+        <v>45013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>